<commit_message>
EPBDS-8913 Rework logging annotations. Tests.
</commit_message>
<xml_diff>
--- a/ITEST/itest.storelogdata/openl-repository/deployments/deployment4/simple4/Main.xlsx
+++ b/ITEST/itest.storelogdata/openl-repository/deployments/deployment4/simple4/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService-WADL-WSDL\openl-repository\deployments\simple1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.storelogdata\openl-repository\deployments\deployment4\simple4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020D7861-BB04-4B62-ACDC-87F6E6C194CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD2F92-B669-490E-9663-2F0607249E55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="90" windowWidth="31815" windowHeight="20565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="1470" windowWidth="28875" windowHeight="17610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -206,12 +206,180 @@
         </r>
       </text>
     </comment>
+    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{9F63C3CC-FDF6-41B9-98F6-483FD6956742}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>This is so-called Decision Table Header. It starts with the keyword "Rules".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{E818964C-EC98-48A2-B0EF-9814A01D826E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Rule column header. Rule column is used to to name particular rule rows for documentation and tracing purposes. It is also useful to create rule rows that span more than one cell vertically (this will be explained in one of the next tutorials)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{9A751868-C512-4A42-8B52-596CED06DC51}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Condition column header. Must start with "C"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{F7471AE5-4603-4933-B83C-3496ACC2F700}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Return column header. Must start with "RET".  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{043BB939-554F-49FA-8783-134637B2F185}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Condition expression. Must have type </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>boolean.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> As you can see condition uses parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve">hour </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>from Method Header and variable</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>that defines column data. When condition is evaluated for each row, the cell value from this row is assigned to variable</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{112E8912-1400-4C57-A470-3E11308067DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">This is return expression performed for the first row where all conditions have been satisfied. The variable </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>greeting</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve"> is substittuted with a cell value from the rule row</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>Rule</t>
   </si>
@@ -292,6 +460,9 @@
   </si>
   <si>
     <t>Value2</t>
+  </si>
+  <si>
+    <t>Rules String Hello2 (Integer hour)</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E21"/>
+  <dimension ref="B3:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1212,10 +1383,127 @@
         <v>16</v>
       </c>
     </row>
+    <row r="27" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+    </row>
+    <row r="28" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0</v>
+      </c>
+      <c r="D32" s="17">
+        <v>11</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="20">
+        <v>12</v>
+      </c>
+      <c r="D33" s="21">
+        <v>17</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="20">
+        <v>18</v>
+      </c>
+      <c r="D34" s="21">
+        <v>21</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="24">
+        <v>22</v>
+      </c>
+      <c r="D35" s="25">
+        <v>23</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B27:E27"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
EPBDS-11982 Support SQL DB for data storage. Tests.
</commit_message>
<xml_diff>
--- a/ITEST/itest.storelogdata/openl-repository/deployments/deployment4/simple4/Main.xlsx
+++ b/ITEST/itest.storelogdata/openl-repository/deployments/deployment4/simple4/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.storelogdata\openl-repository\deployments\deployment4\simple4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\ITEST\itest.storelogdata\openl-repository\deployments\deployment4\simple4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD2F92-B669-490E-9663-2F0607249E55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C9D1A-7F73-40AD-9E03-DA42C77250E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="1470" windowWidth="28875" windowHeight="17610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9970" yWindow="870" windowWidth="25130" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -374,12 +374,180 @@
         </r>
       </text>
     </comment>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{65EFDAA3-C5FF-481A-9F50-FF8E4C9BF624}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>This is so-called Decision Table Header. It starts with the keyword "Rules".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{10F94EF3-28AF-4B27-AB2F-6DBF4C573123}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Rule column header. Rule column is used to to name particular rule rows for documentation and tracing purposes. It is also useful to create rule rows that span more than one cell vertically (this will be explained in one of the next tutorials)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C40" authorId="0" shapeId="0" xr:uid="{32C2384A-1DBC-40AB-9258-FD0E698A1F64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Condition column header. Must start with "C"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E40" authorId="0" shapeId="0" xr:uid="{AED57D61-040C-4483-B3EF-8D0ED63B16C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Return column header. Must start with "RET".  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{8E4BDC0B-F602-47AE-85B9-8C4D73FF04A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Condition expression. Must have type </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>boolean.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> As you can see condition uses parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve">hour </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>from Method Header and variable</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>that defines column data. When condition is evaluated for each row, the cell value from this row is assigned to variable</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E41" authorId="0" shapeId="0" xr:uid="{D6B5CD9D-054D-400F-B4D3-6154730AA049}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">This is return expression performed for the first row where all conditions have been satisfied. The variable </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>greeting</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve"> is substittuted with a cell value from the rule row</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
   <si>
     <t>Rule</t>
   </si>
@@ -463,6 +631,9 @@
   </si>
   <si>
     <t>Rules String Hello2 (Integer hour)</t>
+  </si>
+  <si>
+    <t>Rules String Hello3 (Integer hour)</t>
   </si>
 </sst>
 </file>
@@ -1167,29 +1338,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E35"/>
+  <dimension ref="B3:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
         <v>21</v>
       </c>
@@ -1197,7 +1368,7 @@
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1223,7 +1394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>19</v>
@@ -1235,7 +1406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1448,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
@@ -1291,7 +1462,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>15</v>
       </c>
@@ -1305,7 +1476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1484,7 @@
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
     </row>
-    <row r="17" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="11" t="s">
         <v>23</v>
       </c>
@@ -1327,7 +1498,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>9</v>
       </c>
@@ -1341,7 +1512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
         <v>13</v>
       </c>
@@ -1369,7 +1540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
         <v>15</v>
       </c>
@@ -1383,7 +1554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="27" t="s">
         <v>27</v>
       </c>
@@ -1391,7 +1562,7 @@
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
     </row>
-    <row r="28" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="6" t="s">
         <v>3</v>
@@ -1417,7 +1588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
         <v>19</v>
@@ -1429,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="11" t="s">
         <v>0</v>
       </c>
@@ -1443,7 +1614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
         <v>9</v>
       </c>
@@ -1457,7 +1628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="19" t="s">
         <v>11</v>
       </c>
@@ -1471,7 +1642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="19" t="s">
         <v>13</v>
       </c>
@@ -1485,7 +1656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
         <v>15</v>
       </c>
@@ -1499,11 +1670,128 @@
         <v>16</v>
       </c>
     </row>
+    <row r="39" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+    </row>
+    <row r="40" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="8"/>
+      <c r="C42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0</v>
+      </c>
+      <c r="D44" s="17">
+        <v>11</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="20">
+        <v>12</v>
+      </c>
+      <c r="D45" s="21">
+        <v>17</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="20">
+        <v>18</v>
+      </c>
+      <c r="D46" s="21">
+        <v>21</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="24">
+        <v>22</v>
+      </c>
+      <c r="D47" s="25">
+        <v>23</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B39:E39"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>